<commit_message>
Added xlsx test script
Added zip test script

Added zip file
</commit_message>
<xml_diff>
--- a/src/resources/Document_xlsx.xlsx
+++ b/src/resources/Document_xlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maryg\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maryg\IdeaProjects\files_downloads\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B0D978-71C6-411E-8D19-AD156EA013CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F2B11E-C964-452A-ADB5-2091D15E5250}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0AD189CB-FC74-4A52-983B-90C97DD683EE}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{0AD189CB-FC74-4A52-983B-90C97DD683EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Document_csv" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>get</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>quickly</t>
+  </si>
+  <si>
+    <t>get file quickly</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8C99A0-AA08-4B53-BAE6-8FF2061857CF}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -404,6 +407,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>